<commit_message>
edit: added disclaimer message
</commit_message>
<xml_diff>
--- a/data/raw-data/bangaloreCMP2020Projetcs.xlsx
+++ b/data/raw-data/bangaloreCMP2020Projetcs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\00_Git Repos\bangalore-cmp-2020\data\raw-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D400F17-55C2-4B0F-8698-3E4DCC05FD8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E2509C-B079-4B13-96EF-E85E5C2512FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4275" yWindow="4275" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="73">
   <si>
     <t>id</t>
   </si>
@@ -238,6 +238,12 @@
   </si>
   <si>
     <t>12.952704436325476, 77.60521839559689</t>
+  </si>
+  <si>
+    <t>12.93831866484314, 77.57383860471519</t>
+  </si>
+  <si>
+    <t>12.953047770736154, 77.541725447341</t>
   </si>
 </sst>
 </file>
@@ -558,7 +564,7 @@
   <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,6 +918,9 @@
       <c r="C27" t="s">
         <v>30</v>
       </c>
+      <c r="D27" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
@@ -922,6 +931,9 @@
       </c>
       <c r="C28" t="s">
         <v>31</v>
+      </c>
+      <c r="D28" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add: station area access plan projects
</commit_message>
<xml_diff>
--- a/data/raw-data/bangaloreCMP2020Projetcs.xlsx
+++ b/data/raw-data/bangaloreCMP2020Projetcs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\00_Git Repos\bangalore-cmp-2020\data\raw-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED4EDCD9-FFAB-4D15-9A08-52771BE420FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2614748F-55AB-428B-8487-75411434C837}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4275" yWindow="4275" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="227">
   <si>
     <t>id</t>
   </si>
@@ -619,6 +619,93 @@
   </si>
   <si>
     <t>12.968959086768063, 77.61146152802486</t>
+  </si>
+  <si>
+    <t>Station Area Access Plan</t>
+  </si>
+  <si>
+    <t>Baiyapannahalli Station</t>
+  </si>
+  <si>
+    <t>Yellachanahalli Station</t>
+  </si>
+  <si>
+    <t>Nayandanahalli Station</t>
+  </si>
+  <si>
+    <t>Nagasandra Station</t>
+  </si>
+  <si>
+    <t>Sampige Mantri Square Station</t>
+  </si>
+  <si>
+    <t>Sriramapura Station</t>
+  </si>
+  <si>
+    <t>Rajajinagar Station</t>
+  </si>
+  <si>
+    <t>Mahakavi Kuvempu Road Station</t>
+  </si>
+  <si>
+    <t>Mahalakshmi Station</t>
+  </si>
+  <si>
+    <t>Sandal Soap Factory Station</t>
+  </si>
+  <si>
+    <t>Yeshwantpur Station</t>
+  </si>
+  <si>
+    <t>Peenya Station</t>
+  </si>
+  <si>
+    <t>Peenya Industry Station</t>
+  </si>
+  <si>
+    <t>Dasarahalli Station</t>
+  </si>
+  <si>
+    <t>12.990866321508554, 77.65294454951227</t>
+  </si>
+  <si>
+    <t>12.895860594419416, 77.57004255678578</t>
+  </si>
+  <si>
+    <t>12.946429708785299, 77.52976417747144</t>
+  </si>
+  <si>
+    <t>13.048204340142766, 77.50014317909618</t>
+  </si>
+  <si>
+    <t>12.99057903833429, 77.57085307602627</t>
+  </si>
+  <si>
+    <t>12.9966337716117, 77.56351455573149</t>
+  </si>
+  <si>
+    <t>13.000375243187055, 77.5498452946652</t>
+  </si>
+  <si>
+    <t>12.99852857334125, 77.55704994598644</t>
+  </si>
+  <si>
+    <t>13.008238795034371, 77.54894763067821</t>
+  </si>
+  <si>
+    <t>13.014845877265085, 77.55412978470413</t>
+  </si>
+  <si>
+    <t>13.023334344199698, 77.54960785891855</t>
+  </si>
+  <si>
+    <t>13.036495649964248, 77.52539754228509</t>
+  </si>
+  <si>
+    <t>13.032955134958728, 77.53343784692174</t>
+  </si>
+  <si>
+    <t>13.043586550497832, 77.51250107757342</t>
   </si>
 </sst>
 </file>
@@ -936,17 +1023,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F265"/>
+  <dimension ref="A1:F279"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A235" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F265" sqref="F265"/>
+      <selection pane="bottomLeft" activeCell="F280" sqref="F280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="37" bestFit="1" customWidth="1"/>
@@ -3966,6 +4053,202 @@
         <v>200</v>
       </c>
     </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A266">
+        <v>4001</v>
+      </c>
+      <c r="B266" t="s">
+        <v>198</v>
+      </c>
+      <c r="C266" t="s">
+        <v>199</v>
+      </c>
+      <c r="F266" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A267">
+        <v>4002</v>
+      </c>
+      <c r="B267" t="s">
+        <v>198</v>
+      </c>
+      <c r="C267" t="s">
+        <v>200</v>
+      </c>
+      <c r="F267" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A268">
+        <v>4003</v>
+      </c>
+      <c r="B268" t="s">
+        <v>198</v>
+      </c>
+      <c r="C268" t="s">
+        <v>201</v>
+      </c>
+      <c r="F268" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A269">
+        <v>4004</v>
+      </c>
+      <c r="B269" t="s">
+        <v>198</v>
+      </c>
+      <c r="C269" t="s">
+        <v>202</v>
+      </c>
+      <c r="F269" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A270">
+        <v>4005</v>
+      </c>
+      <c r="B270" t="s">
+        <v>198</v>
+      </c>
+      <c r="C270" t="s">
+        <v>203</v>
+      </c>
+      <c r="F270" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A271">
+        <v>4006</v>
+      </c>
+      <c r="B271" t="s">
+        <v>198</v>
+      </c>
+      <c r="C271" t="s">
+        <v>204</v>
+      </c>
+      <c r="F271" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A272">
+        <v>4007</v>
+      </c>
+      <c r="B272" t="s">
+        <v>198</v>
+      </c>
+      <c r="C272" t="s">
+        <v>205</v>
+      </c>
+      <c r="F272" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A273">
+        <v>4008</v>
+      </c>
+      <c r="B273" t="s">
+        <v>198</v>
+      </c>
+      <c r="C273" t="s">
+        <v>206</v>
+      </c>
+      <c r="F273" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A274">
+        <v>4009</v>
+      </c>
+      <c r="B274" t="s">
+        <v>198</v>
+      </c>
+      <c r="C274" t="s">
+        <v>207</v>
+      </c>
+      <c r="F274" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A275">
+        <v>4010</v>
+      </c>
+      <c r="B275" t="s">
+        <v>198</v>
+      </c>
+      <c r="C275" t="s">
+        <v>208</v>
+      </c>
+      <c r="F275" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A276">
+        <v>4011</v>
+      </c>
+      <c r="B276" t="s">
+        <v>198</v>
+      </c>
+      <c r="C276" t="s">
+        <v>209</v>
+      </c>
+      <c r="F276" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A277">
+        <v>4012</v>
+      </c>
+      <c r="B277" t="s">
+        <v>198</v>
+      </c>
+      <c r="C277" t="s">
+        <v>210</v>
+      </c>
+      <c r="F277" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A278">
+        <v>4013</v>
+      </c>
+      <c r="B278" t="s">
+        <v>198</v>
+      </c>
+      <c r="C278" t="s">
+        <v>211</v>
+      </c>
+      <c r="F278" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A279">
+        <v>4014</v>
+      </c>
+      <c r="B279" t="s">
+        <v>198</v>
+      </c>
+      <c r="C279" t="s">
+        <v>212</v>
+      </c>
+      <c r="F279" t="s">
+        <v>226</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add: Station Area Access Plans Analysis Page; Draft 0
</commit_message>
<xml_diff>
--- a/data/raw-data/bangaloreCMP2020Projetcs.xlsx
+++ b/data/raw-data/bangaloreCMP2020Projetcs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\00_Git Repos\bangalore-cmp-2020\data\raw-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2614748F-55AB-428B-8487-75411434C837}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB427BB4-629D-4050-83EC-2D735C7AE0EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4275" yWindow="4275" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1026,9 +1026,9 @@
   <dimension ref="A1:F279"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A235" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A236" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F280" sqref="F280"/>
+      <selection pane="bottomLeft" activeCell="N249" sqref="N249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>